<commit_message>
regression in matlab and fitting in python
</commit_message>
<xml_diff>
--- a/data/temperature25.xlsx
+++ b/data/temperature25.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\Git_Repositories\Semester_Thesis_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2217518-8DC7-407F-B993-78A964B5103C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E84DED-140B-4C5F-8C7B-E415B89590D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1725" windowWidth="29040" windowHeight="15720" xr2:uid="{FD10B2A9-E45B-4928-8984-6B25599DFDFD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{FD10B2A9-E45B-4928-8984-6B25599DFDFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,10 @@
     <t>Current_A</t>
   </si>
   <si>
-    <t>QC_W</t>
+    <t>Qremoved_W</t>
   </si>
   <si>
-    <t>Qh_W</t>
+    <t>Qwaste_W</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>